<commit_message>
Added readme_but still in process of editing
</commit_message>
<xml_diff>
--- a/figures/Uncertainty_MS_2018/Table_ Uncertainty MS_2018.xlsx
+++ b/figures/Uncertainty_MS_2018/Table_ Uncertainty MS_2018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="2380" windowWidth="40500" windowHeight="19180" tabRatio="500"/>
+    <workbookView xWindow="-60" yWindow="-80" windowWidth="23500" windowHeight="25000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="51">
   <si>
     <r>
       <t>American lobster (</t>
@@ -280,17 +280,28 @@
     <t>TSS(max)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>Probability of occurrence model</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biomass model</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inter. Depth</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -332,12 +343,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,21 +689,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:AB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="3" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -1843,6 +1863,16 @@
       </c>
     </row>
     <row r="29" spans="1:28">
+      <c r="B29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
       <c r="P29" s="2" t="s">
         <v>11</v>
       </c>
@@ -1869,11 +1899,53 @@
       </c>
     </row>
     <row r="30" spans="1:28">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="P30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:28">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="8">
+        <v>10050</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D31" s="7">
+        <v>10</v>
+      </c>
+      <c r="E31" s="7">
+        <v>7750</v>
+      </c>
+      <c r="F31" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G31" s="9">
+        <v>10</v>
+      </c>
       <c r="P31" t="s">
         <v>9</v>
       </c>
@@ -1900,6 +1972,27 @@
       </c>
     </row>
     <row r="32" spans="1:28">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="8">
+        <v>6550</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D32" s="7">
+        <v>10</v>
+      </c>
+      <c r="E32" s="7">
+        <v>10050</v>
+      </c>
+      <c r="F32" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G32" s="9">
+        <v>10</v>
+      </c>
       <c r="P32" t="s">
         <v>10</v>
       </c>
@@ -1925,7 +2018,28 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="16:23">
+    <row r="33" spans="1:23">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="8">
+        <v>7550</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D33" s="7">
+        <v>10</v>
+      </c>
+      <c r="E33" s="7">
+        <v>2950</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="G33" s="9">
+        <v>10</v>
+      </c>
       <c r="P33" s="2" t="s">
         <v>11</v>
       </c>
@@ -1951,12 +2065,54 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="34" spans="16:23">
+    <row r="34" spans="1:23">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="8">
+        <v>8550</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D34" s="7">
+        <v>10</v>
+      </c>
+      <c r="E34" s="7">
+        <v>4850</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="G34" s="9">
+        <v>10</v>
+      </c>
       <c r="P34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="16:23">
+    <row r="35" spans="1:23">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="8">
+        <v>6050</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D35" s="7">
+        <v>10</v>
+      </c>
+      <c r="E35" s="7">
+        <v>6350</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="G35" s="9">
+        <v>10</v>
+      </c>
       <c r="P35" t="s">
         <v>9</v>
       </c>
@@ -1982,7 +2138,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="16:23">
+    <row r="36" spans="1:23">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="8">
+        <v>3050</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D36" s="7">
+        <v>10</v>
+      </c>
+      <c r="E36" s="7">
+        <v>2650</v>
+      </c>
+      <c r="F36" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G36" s="9">
+        <v>10</v>
+      </c>
       <c r="P36" s="2" t="s">
         <v>10</v>
       </c>
@@ -2008,7 +2185,28 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="37" spans="16:23">
+    <row r="37" spans="1:23">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="8">
+        <v>7550</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D37" s="7">
+        <v>8</v>
+      </c>
+      <c r="E37" s="7">
+        <v>5050</v>
+      </c>
+      <c r="F37" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G37" s="9">
+        <v>8</v>
+      </c>
       <c r="P37" t="s">
         <v>11</v>
       </c>
@@ -2034,7 +2232,25 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
+    <row r="39" spans="1:23">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="42" spans="1:23">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="45" spans="1:23">
+      <c r="D45" s="2"/>
+    </row>
+    <row r="47" spans="1:23">
+      <c r="D47" s="2"/>
+    </row>
+    <row r="51" spans="4:4">
+      <c r="D51" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E29:G29"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update to README file
</commit_message>
<xml_diff>
--- a/figures/Uncertainty_MS_2018/Table_ Uncertainty MS_2018.xlsx
+++ b/figures/Uncertainty_MS_2018/Table_ Uncertainty MS_2018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-80" windowWidth="23500" windowHeight="25000" tabRatio="500"/>
+    <workbookView xWindow="26580" yWindow="-80" windowWidth="23500" windowHeight="25000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
+  <si>
+    <t>2.1 Modeled Species</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.2 Survey and Environmental Data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3 Species Niche Modeling</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.4 Projecting Species Habitat Distribution</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5 Analyses</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 RESULTS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1 Partitioning Projection Uncertainty</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3 Ensemble Projections with RCP 8.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 DISCUSSION</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1 Characterizing Uncertainty in Species Projections</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2 Projected shifts in habitat for important resource species</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 CONCLUSIONS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACKNOWLEDGEMENTS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>REFERENCES</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUPPORTING INFORMATION</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2 Niche Model Comparisons with RCP 8.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 INTRODUCTION</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 MATERIALS AND METHODS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <r>
       <t>American lobster (</t>
@@ -303,7 +375,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -321,6 +393,15 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="2">
@@ -343,13 +424,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -360,6 +440,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,7 +775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -717,100 +803,108 @@
     <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.7109375" customWidth="1"/>
     <col min="23" max="23" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:27">
       <c r="G1" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
       <c r="V1" s="3" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23">
-      <c r="A3" t="s">
-        <v>8</v>
       </c>
       <c r="B3">
         <v>19437</v>
@@ -819,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G3" s="3">
         <v>0.32</v>
@@ -843,12 +937,18 @@
         <v>0.71</v>
       </c>
       <c r="P3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23">
+        <v>21</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15">
       <c r="D4" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3">
         <v>0.33</v>
@@ -872,7 +972,7 @@
         <v>0.72</v>
       </c>
       <c r="P4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="3">
         <v>0.32</v>
@@ -895,16 +995,22 @@
       <c r="W4" s="3">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="Z4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15">
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="G5" s="3">
         <v>0.4</v>
@@ -928,7 +1034,7 @@
         <v>0.75</v>
       </c>
       <c r="P5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="3">
         <v>0.33</v>
@@ -951,10 +1057,13 @@
       <c r="W5" s="3">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="Z5" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>8349</v>
@@ -963,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G6" s="3">
         <v>0.36</v>
@@ -987,7 +1096,7 @@
         <v>0.97</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="Q6" s="3">
         <v>0.4</v>
@@ -1010,10 +1119,13 @@
       <c r="W6" s="4">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="Z6" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="15">
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="G7" s="3">
         <v>0.38</v>
@@ -1037,18 +1149,21 @@
         <v>0.98</v>
       </c>
       <c r="P7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23">
+        <v>20</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="15">
       <c r="D8" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G8" s="3">
         <v>0.47</v>
@@ -1072,7 +1187,7 @@
         <v>0.92</v>
       </c>
       <c r="P8" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="3">
         <v>0.36</v>
@@ -1095,10 +1210,13 @@
       <c r="W8" s="3">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="Z8" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>13291</v>
@@ -1107,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G9" s="3">
         <v>0.45</v>
@@ -1131,7 +1249,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="Q9" s="3">
         <v>0.38</v>
@@ -1154,10 +1272,13 @@
       <c r="W9" s="4">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="Z9" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="15">
       <c r="D10" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G10" s="3">
         <v>0.46</v>
@@ -1181,7 +1302,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="P10" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="Q10" s="3">
         <v>0.47</v>
@@ -1204,16 +1325,19 @@
       <c r="W10" s="3">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="Z10" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="15">
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="G11" s="3">
         <v>0.52</v>
@@ -1237,12 +1361,15 @@
         <v>0.27</v>
       </c>
       <c r="P11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
+        <v>19</v>
+      </c>
+      <c r="Z11" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="15">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>2588</v>
@@ -1251,7 +1378,7 @@
         <v>518</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G12" s="3">
         <v>0.44</v>
@@ -1275,7 +1402,7 @@
         <v>0.38</v>
       </c>
       <c r="P12" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="Q12" s="3">
         <v>0.4</v>
@@ -1298,10 +1425,13 @@
       <c r="W12" s="3">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="Z12" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
       <c r="D13" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G13" s="3">
         <v>0.45</v>
@@ -1325,7 +1455,7 @@
         <v>0.15</v>
       </c>
       <c r="P13" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="Q13" s="3">
         <v>0.46</v>
@@ -1348,16 +1478,19 @@
       <c r="W13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="Z13" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="15">
       <c r="D14" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="G14" s="3">
         <v>0.52</v>
@@ -1381,7 +1514,7 @@
         <v>0.15</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="Q14" s="3">
         <v>0.54</v>
@@ -1404,10 +1537,13 @@
       <c r="W14" s="3">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="15" spans="1:23">
+      <c r="Z14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="15">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>12121</v>
@@ -1416,7 +1552,7 @@
         <v>3183</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G15" s="3">
         <v>0.26</v>
@@ -1440,12 +1576,15 @@
         <v>0.76</v>
       </c>
       <c r="P15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23">
+        <v>18</v>
+      </c>
+      <c r="Z15" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="D16" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G16" s="3">
         <v>0.3</v>
@@ -1469,7 +1608,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="P16" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="Q16" s="3">
         <v>0.26</v>
@@ -1492,16 +1631,19 @@
       <c r="W16" s="3">
         <v>0.76</v>
       </c>
+      <c r="Z16" s="12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:28">
       <c r="D17" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="G17" s="3">
         <v>0.42</v>
@@ -1525,7 +1667,7 @@
         <v>0.85</v>
       </c>
       <c r="P17" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="Q17" s="3">
         <v>0.3</v>
@@ -1548,10 +1690,13 @@
       <c r="W17" s="3">
         <v>0.28999999999999998</v>
       </c>
+      <c r="Z17" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:28">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>5282</v>
@@ -1560,7 +1705,7 @@
         <v>1570</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G18" s="3">
         <v>0.28000000000000003</v>
@@ -1584,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="Q18" s="3">
         <v>0.42</v>
@@ -1607,10 +1752,13 @@
       <c r="W18" s="3">
         <v>0.85</v>
       </c>
+      <c r="Z18" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19" spans="1:28">
       <c r="D19" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="G19" s="3">
         <v>0.33</v>
@@ -1633,16 +1781,19 @@
       <c r="M19" s="3">
         <v>0.18</v>
       </c>
+      <c r="Z19" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="20" spans="1:28">
       <c r="D20" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="G20" s="3">
         <v>0.42</v>
@@ -1668,7 +1819,7 @@
     </row>
     <row r="21" spans="1:28">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B21">
         <v>12281</v>
@@ -1677,7 +1828,7 @@
         <v>2970</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G21" s="3">
         <v>0.4</v>
@@ -1703,7 +1854,7 @@
     </row>
     <row r="22" spans="1:28">
       <c r="D22" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G22" s="3">
         <v>0.46</v>
@@ -1729,13 +1880,13 @@
     </row>
     <row r="23" spans="1:28">
       <c r="D23" s="2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="G23" s="3">
         <v>0.54</v>
@@ -1761,16 +1912,16 @@
     </row>
     <row r="24" spans="1:28">
       <c r="Q24" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="R24" s="3"/>
       <c r="S24" s="3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
@@ -1781,38 +1932,38 @@
     </row>
     <row r="25" spans="1:28">
       <c r="P25" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="U25" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="V25" s="3" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:28">
       <c r="P26" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:28">
       <c r="P27" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="Q27" s="3">
         <v>0.45</v>
@@ -1838,7 +1989,7 @@
     </row>
     <row r="28" spans="1:28">
       <c r="P28" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="Q28" s="3">
         <v>0.46</v>
@@ -1863,18 +2014,18 @@
       </c>
     </row>
     <row r="29" spans="1:28">
-      <c r="B29" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
       <c r="P29" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="Q29" s="3">
         <v>0.52</v>
@@ -1900,54 +2051,54 @@
     </row>
     <row r="30" spans="1:28">
       <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>50</v>
+      <c r="B30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="P30" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:28">
       <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="8">
+        <v>26</v>
+      </c>
+      <c r="B31" s="7">
         <v>10050</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <v>0.01</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>10</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>7750</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="8">
         <v>10</v>
       </c>
       <c r="P31" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="Q31" s="3">
         <v>0.44</v>
@@ -1973,28 +2124,28 @@
     </row>
     <row r="32" spans="1:28">
       <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="8">
+        <v>37</v>
+      </c>
+      <c r="B32" s="7">
         <v>6550</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="7">
         <v>0.02</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>10</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>10050</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="8">
         <v>10</v>
       </c>
       <c r="P32" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="Q32" s="3">
         <v>0.45</v>
@@ -2020,28 +2171,28 @@
     </row>
     <row r="33" spans="1:23">
       <c r="A33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="8">
+        <v>42</v>
+      </c>
+      <c r="B33" s="7">
         <v>7550</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>0.02</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="6">
         <v>10</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="6">
         <v>2950</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="6">
         <v>0.01</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="8">
         <v>10</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="Q33" s="3">
         <v>0.52</v>
@@ -2067,54 +2218,54 @@
     </row>
     <row r="34" spans="1:23">
       <c r="A34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="8">
+        <v>40</v>
+      </c>
+      <c r="B34" s="7">
         <v>8550</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <v>0.02</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>10</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>4850</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>0.01</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="8">
         <v>10</v>
       </c>
       <c r="P34" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:23">
       <c r="A35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="8">
+        <v>38</v>
+      </c>
+      <c r="B35" s="7">
         <v>6050</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="7">
         <v>0.02</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <v>10</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>6350</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="6">
         <v>0.01</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="8">
         <v>10</v>
       </c>
       <c r="P35" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="Q35" s="3">
         <v>0.28000000000000003</v>
@@ -2140,28 +2291,28 @@
     </row>
     <row r="36" spans="1:23">
       <c r="A36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B36" s="8">
+        <v>39</v>
+      </c>
+      <c r="B36" s="7">
         <v>3050</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="7">
         <v>0.02</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="6">
         <v>10</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
         <v>2650</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="8">
         <v>10</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="Q36" s="3">
         <v>0.33</v>
@@ -2187,28 +2338,28 @@
     </row>
     <row r="37" spans="1:23">
       <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="8">
+        <v>41</v>
+      </c>
+      <c r="B37" s="7">
         <v>7550</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <v>0.02</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="6">
         <v>8</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>5050</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="8">
         <v>8</v>
       </c>
       <c r="P37" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="Q37" s="3">
         <v>0.42</v>

</xml_diff>